<commit_message>
added notes on required changes
</commit_message>
<xml_diff>
--- a/xls/templates/run-rate-template.xlsx
+++ b/xls/templates/run-rate-template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BDA0C5-565E-2B4F-B1C9-E245EA5D0405}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DE20C7-AF93-FA4F-92B1-F912DE251932}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="460" windowWidth="38380" windowHeight="21060" activeTab="1" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="1" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
   <si>
     <t>Start Date</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>Average Weekly Move Outs</t>
+  </si>
+  <si>
+    <t>Notice to Renew</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -678,6 +681,47 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="14" borderId="0" xfId="16" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="17"/>
+    <xf numFmtId="164" fontId="8" fillId="15" borderId="0" xfId="17" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="3" fillId="2" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="14" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -737,47 +781,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="13" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="7" fillId="14" borderId="0" xfId="16" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="17"/>
-    <xf numFmtId="164" fontId="8" fillId="15" borderId="0" xfId="17" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="3" fillId="2" borderId="0" xfId="4" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -1137,18 +1140,18 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="25" t="s">
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -4434,16 +4437,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4156A3-96B9-DE41-91DB-F4C9577E214C}">
-  <dimension ref="A1:Y72"/>
+  <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="E27" sqref="E26:E27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="101" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="59" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="39" customWidth="1"/>
     <col min="4" max="4" width="24.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="11" max="11" width="10.6640625" customWidth="1"/>
@@ -4452,48 +4455,50 @@
     <col min="17" max="17" width="6.6640625" customWidth="1"/>
     <col min="18" max="18" width="14.1640625" customWidth="1"/>
     <col min="19" max="19" width="9.83203125" customWidth="1"/>
-    <col min="20" max="20" width="9.5" customWidth="1"/>
-    <col min="21" max="21" width="22" customWidth="1"/>
-    <col min="22" max="22" width="15.33203125" customWidth="1"/>
-    <col min="24" max="24" width="14.5" customWidth="1"/>
-    <col min="25" max="25" width="16" customWidth="1"/>
+    <col min="20" max="20" width="14" customWidth="1"/>
+    <col min="21" max="21" width="9.5" customWidth="1"/>
+    <col min="22" max="22" width="22" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" customWidth="1"/>
+    <col min="25" max="25" width="14.5" customWidth="1"/>
+    <col min="26" max="26" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="D1" s="30" t="s">
+      <c r="B1" s="46"/>
+      <c r="D1" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="G1" s="30" t="s">
+      <c r="E1" s="47"/>
+      <c r="G1" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="K1" s="31" t="s">
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="K1" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-    </row>
-    <row r="2" spans="1:25" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+    </row>
+    <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="49"/>
+      <c r="B2" s="29"/>
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -4535,29 +4540,32 @@
         <v>96</v>
       </c>
       <c r="T2" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="U2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="V2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="W2" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="X2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="Y2" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Z2" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="56"/>
       <c r="D3" t="s">
         <v>85</v>
       </c>
@@ -4570,35 +4578,35 @@
       <c r="H3" s="13">
         <v>0.14299999999999999</v>
       </c>
-      <c r="I3" s="47">
+      <c r="I3" s="27">
         <f>H3</f>
         <v>0.14299999999999999</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <f>$E$4</f>
         <v>163</v>
       </c>
-      <c r="W3" s="8">
-        <f>V3/$E$3</f>
+      <c r="X3" s="8">
+        <f>W3/$E$3</f>
         <v>0.61977186311787069</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <f>$E$8</f>
         <v>147</v>
       </c>
-      <c r="Y3" s="8">
-        <f>X3/$E$3</f>
+      <c r="Z3" s="8">
+        <f>Y3/$E$3</f>
         <v>0.55893536121673004</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="29" t="s">
         <v>60</v>
       </c>
       <c r="D4" t="s">
@@ -4613,7 +4621,7 @@
       <c r="H4" s="8">
         <v>0.31</v>
       </c>
-      <c r="I4" s="47">
+      <c r="I4" s="27">
         <f t="shared" ref="I4:I7" si="0">H4</f>
         <v>0.31</v>
       </c>
@@ -4654,34 +4662,38 @@
         <v>0</v>
       </c>
       <c r="T4" s="3">
+        <f>U7</f>
         <v>0</v>
       </c>
       <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
         <f ca="1">Q4-S4</f>
         <v>5</v>
       </c>
-      <c r="V4" s="16">
-        <f ca="1">V3+U4</f>
+      <c r="W4" s="16">
+        <f ca="1">W3+V4</f>
         <v>168</v>
       </c>
-      <c r="W4" s="8">
-        <f t="shared" ref="W4:W37" ca="1" si="1">V4/$E$3</f>
+      <c r="X4" s="8">
+        <f t="shared" ref="X4:X37" ca="1" si="1">W4/$E$3</f>
         <v>0.63878326996197721</v>
       </c>
-      <c r="X4" s="3">
-        <f ca="1">X3+Q4-S4</f>
+      <c r="Y4" s="3">
+        <f ca="1">Y3+Q4-S4</f>
         <v>152</v>
       </c>
-      <c r="Y4" s="8">
-        <f t="shared" ref="Y4:Y37" ca="1" si="2">X4/$E$3</f>
+      <c r="Z4" s="8">
+        <f t="shared" ref="Z4:Z37" ca="1" si="2">Y4/$E$3</f>
         <v>0.57794676806083645</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="50">
+      <c r="B5" s="30">
         <v>43542</v>
       </c>
       <c r="D5" t="s">
@@ -4696,7 +4708,7 @@
       <c r="H5" s="8">
         <v>0.35</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="27">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
@@ -4737,41 +4749,45 @@
         <v>0</v>
       </c>
       <c r="T5" s="3">
+        <f t="shared" ref="T5:T36" si="10">U8</f>
         <v>0</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" ref="U5:U13" ca="1" si="10">Q5-S5</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <f t="shared" ref="V5:V13" ca="1" si="11">Q5-S5</f>
         <v>5</v>
       </c>
-      <c r="V5" s="16">
-        <f t="shared" ref="V5:V37" ca="1" si="11">V4+U5</f>
+      <c r="W5" s="16">
+        <f t="shared" ref="W5:W37" ca="1" si="12">W4+V5</f>
         <v>173</v>
       </c>
-      <c r="W5" s="8">
+      <c r="X5" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.65779467680608361</v>
       </c>
-      <c r="X5" s="3">
-        <f t="shared" ref="X5:X37" ca="1" si="12">X4+Q5-S5</f>
+      <c r="Y5" s="3">
+        <f t="shared" ref="Y5:Y37" ca="1" si="13">Y4+Q5-S5</f>
         <v>157</v>
       </c>
-      <c r="Y5" s="8">
+      <c r="Z5" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.59695817490494296</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="50">
+      <c r="B6" s="30">
         <f ca="1">INDIRECT("K"&amp;E9)</f>
         <v>43689</v>
       </c>
       <c r="D6" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="46">
+      <c r="E6" s="26">
         <f>ROUND(E3*E5,0)</f>
         <v>237</v>
       </c>
@@ -4781,13 +4797,13 @@
       <c r="H6" s="8">
         <v>0.85</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="27">
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="15">
-        <f t="shared" ref="K6:K11" si="13">K5+7</f>
+        <f t="shared" ref="K6:K11" si="14">K5+7</f>
         <v>43563</v>
       </c>
       <c r="L6" s="3">
@@ -4822,41 +4838,45 @@
         <v>0</v>
       </c>
       <c r="T6" s="3">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="U6" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V6" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>5</v>
       </c>
-      <c r="V6" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W6" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>178</v>
       </c>
-      <c r="W6" s="8">
+      <c r="X6" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.67680608365019013</v>
       </c>
-      <c r="X6" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y6" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>162</v>
       </c>
-      <c r="Y6" s="8">
+      <c r="Z6" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.61596958174904948</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="40">
         <f ca="1">B47/B8</f>
         <v>3.8095238095238092E-2</v>
       </c>
       <c r="D7" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="26">
         <f ca="1">Baseline!R4/COUNT(Baseline!R5:INDIRECT("Baseline!R"&amp;Baseline!B1))</f>
         <v>400</v>
       </c>
@@ -4866,13 +4886,13 @@
       <c r="H7" s="12">
         <v>0.46</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="27">
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>43570</v>
       </c>
       <c r="L7" s="3">
@@ -4907,34 +4927,38 @@
         <v>0</v>
       </c>
       <c r="T7" s="3">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="U7" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>5</v>
       </c>
-      <c r="V7" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W7" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>183</v>
       </c>
-      <c r="W7" s="8">
+      <c r="X7" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.69581749049429653</v>
       </c>
-      <c r="X7" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y7" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>167</v>
       </c>
-      <c r="Y7" s="8">
+      <c r="Z7" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.63498098859315588</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="32">
         <f>$E$11</f>
         <v>1000</v>
       </c>
@@ -4949,7 +4973,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>43577</v>
       </c>
       <c r="L8" s="3">
@@ -4984,32 +5008,36 @@
         <v>0</v>
       </c>
       <c r="T8" s="3">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>5</v>
       </c>
-      <c r="V8" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W8" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>188</v>
       </c>
-      <c r="W8" s="8">
+      <c r="X8" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.71482889733840305</v>
       </c>
-      <c r="X8" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y8" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>172</v>
       </c>
-      <c r="Y8" s="8">
+      <c r="Z8" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.6539923954372624</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="53"/>
+      <c r="B9" s="33"/>
       <c r="D9" t="s">
         <v>109</v>
       </c>
@@ -5021,7 +5049,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>43584</v>
       </c>
       <c r="L9" s="3">
@@ -5056,38 +5084,42 @@
         <v>0</v>
       </c>
       <c r="T9" s="3">
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="U9" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>5</v>
       </c>
-      <c r="V9" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W9" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>193</v>
       </c>
-      <c r="W9" s="8">
+      <c r="X9" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.73384030418250945</v>
       </c>
-      <c r="X9" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y9" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>177</v>
       </c>
-      <c r="Y9" s="8">
+      <c r="Z9" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.6730038022813688</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="33"/>
+      <c r="B10" s="50"/>
       <c r="D10" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="25">
         <f ca="1">COUNT(K4:INDIRECT("K"&amp;E9))</f>
         <v>21</v>
       </c>
@@ -5096,7 +5128,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>43591</v>
       </c>
       <c r="L10" s="3">
@@ -5131,41 +5163,45 @@
         <v>0</v>
       </c>
       <c r="T10" s="3">
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="U10" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V10" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>5</v>
       </c>
-      <c r="V10" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W10" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>198</v>
       </c>
-      <c r="W10" s="8">
+      <c r="X10" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.75285171102661597</v>
       </c>
-      <c r="X10" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y10" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>182</v>
       </c>
-      <c r="Y10" s="8">
+      <c r="Z10" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.69201520912547532</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="49">
-        <f ca="1">INDIRECT("V"&amp;E9)-V3</f>
-        <v>74</v>
+      <c r="B11" s="29">
+        <f ca="1">INDIRECT("V"&amp;E9)-W3</f>
+        <v>-163</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="48">
+      <c r="E11" s="28">
         <v>1000</v>
       </c>
       <c r="G11" s="15"/>
@@ -5173,7 +5209,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>43598</v>
       </c>
       <c r="L11" s="3">
@@ -5208,40 +5244,44 @@
         <v>0</v>
       </c>
       <c r="T11" s="3">
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="U11" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>5</v>
       </c>
-      <c r="V11" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W11" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>203</v>
       </c>
-      <c r="W11" s="8">
+      <c r="X11" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.77186311787072248</v>
       </c>
-      <c r="X11" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y11" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>187</v>
       </c>
-      <c r="Y11" s="8">
+      <c r="Z11" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.71102661596958172</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="49">
+      <c r="B12" s="29">
         <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="24">
         <f ca="1">Baseline!B4/COUNT(Baseline!A5:INDIRECT("Baseline!A"&amp;Baseline!B1))</f>
         <v>0.2857142857142857</v>
       </c>
@@ -5285,34 +5325,38 @@
         <v>2</v>
       </c>
       <c r="T12" s="3">
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="U12" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="V12" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>3</v>
       </c>
-      <c r="V12" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W12" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>206</v>
       </c>
-      <c r="W12" s="8">
+      <c r="X12" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.78326996197718635</v>
       </c>
-      <c r="X12" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y12" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>190</v>
       </c>
-      <c r="Y12" s="8">
+      <c r="Z12" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.72243346007604559</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="51">
+      <c r="B13" s="31">
         <f ca="1">B12/B42</f>
         <v>8.7301587301587297E-2</v>
       </c>
@@ -5357,43 +5401,47 @@
         <v>2</v>
       </c>
       <c r="T13" s="3">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="U13" s="3">
-        <f t="shared" ca="1" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="V13" s="3">
+        <f t="shared" ca="1" si="11"/>
         <v>3</v>
       </c>
-      <c r="V13" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W13" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>209</v>
       </c>
-      <c r="W13" s="8">
+      <c r="X13" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.79467680608365021</v>
       </c>
-      <c r="X13" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y13" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>193</v>
       </c>
-      <c r="Y13" s="8">
+      <c r="Z13" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.73384030418250945</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="49">
-        <f ca="1">SUM(T4:INDIRECT("S"&amp;E9))</f>
-        <v>58</v>
+      <c r="B14" s="29">
+        <f ca="1">SUM(U4:INDIRECT("S"&amp;E9))</f>
+        <v>91</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="15">
-        <f t="shared" ref="K14:K18" si="14">K13+7</f>
+        <f t="shared" ref="K14:K18" si="15">K13+7</f>
         <v>43619</v>
       </c>
       <c r="L14" s="3">
@@ -5428,36 +5476,40 @@
         <v>2</v>
       </c>
       <c r="T14" s="3">
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="U14" s="3">
+        <v>2</v>
+      </c>
+      <c r="V14" s="3">
         <f ca="1">Q14-S14</f>
         <v>3</v>
       </c>
-      <c r="V14" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W14" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>212</v>
       </c>
-      <c r="W14" s="8">
+      <c r="X14" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.80608365019011408</v>
       </c>
-      <c r="X14" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y14" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>196</v>
       </c>
-      <c r="Y14" s="8">
+      <c r="Z14" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.74524714828897343</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="49">
+      <c r="B15" s="29">
         <f ca="1">B14</f>
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -5467,7 +5519,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>43626</v>
       </c>
       <c r="L15" s="3">
@@ -5502,36 +5554,40 @@
         <v>2</v>
       </c>
       <c r="T15" s="3">
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="U15" s="3">
-        <f t="shared" ref="U15:U18" ca="1" si="15">Q15-S15</f>
+        <v>2</v>
+      </c>
+      <c r="V15" s="3">
+        <f t="shared" ref="V15:V18" ca="1" si="16">Q15-S15</f>
         <v>3</v>
       </c>
-      <c r="V15" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W15" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>215</v>
       </c>
-      <c r="W15" s="8">
+      <c r="X15" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.81749049429657794</v>
       </c>
-      <c r="X15" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y15" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>199</v>
       </c>
-      <c r="Y15" s="8">
+      <c r="Z15" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.75665399239543729</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="51">
+      <c r="B16" s="31">
         <f ca="1">B15/B17</f>
-        <v>0.61052631578947369</v>
+        <v>0.7109375</v>
       </c>
       <c r="D16" t="s">
         <v>113</v>
@@ -5541,7 +5597,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>43633</v>
       </c>
       <c r="L16" s="3">
@@ -5576,36 +5632,40 @@
         <v>2</v>
       </c>
       <c r="T16" s="3">
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="U16" s="3">
-        <f t="shared" ca="1" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="V16" s="3">
+        <f t="shared" ca="1" si="16"/>
         <v>3</v>
       </c>
-      <c r="V16" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W16" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>218</v>
       </c>
-      <c r="W16" s="8">
+      <c r="X16" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.82889733840304181</v>
       </c>
-      <c r="X16" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y16" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>202</v>
       </c>
-      <c r="Y16" s="8">
+      <c r="Z16" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.76806083650190116</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="29">
         <f ca="1">B18+B15</f>
-        <v>95</v>
+        <v>128</v>
       </c>
       <c r="D17" t="s">
         <v>114</v>
@@ -5615,7 +5675,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>43640</v>
       </c>
       <c r="L17" s="3">
@@ -5650,34 +5710,38 @@
         <v>2</v>
       </c>
       <c r="T17" s="3">
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="U17" s="3">
-        <f t="shared" ca="1" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="V17" s="3">
+        <f t="shared" ca="1" si="16"/>
         <v>3</v>
       </c>
-      <c r="V17" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W17" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>221</v>
       </c>
-      <c r="W17" s="8">
+      <c r="X17" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.84030418250950567</v>
       </c>
-      <c r="X17" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y17" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>205</v>
       </c>
-      <c r="Y17" s="8">
+      <c r="Z17" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.77946768060836502</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="49">
+      <c r="B18" s="29">
         <f ca="1">SUM(R4:INDIRECT("R"&amp;E9))</f>
         <v>37</v>
       </c>
@@ -5686,7 +5750,7 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>43647</v>
       </c>
       <c r="L18" s="3">
@@ -5721,34 +5785,38 @@
         <v>2</v>
       </c>
       <c r="T18" s="3">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>3</v>
       </c>
       <c r="U18" s="3">
-        <f t="shared" ca="1" si="15"/>
+        <v>2</v>
+      </c>
+      <c r="V18" s="3">
+        <f t="shared" ca="1" si="16"/>
         <v>3</v>
       </c>
-      <c r="V18" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W18" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>224</v>
       </c>
-      <c r="W18" s="8">
+      <c r="X18" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.85171102661596954</v>
       </c>
-      <c r="X18" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y18" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>208</v>
       </c>
-      <c r="Y18" s="8">
+      <c r="Z18" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.79087452471482889</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="54">
+      <c r="B19" s="34">
         <v>0.9</v>
       </c>
       <c r="G19" s="15"/>
@@ -5791,34 +5859,38 @@
         <v>1</v>
       </c>
       <c r="T19" s="3">
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="U19" s="3">
+        <v>1</v>
+      </c>
+      <c r="V19" s="3">
         <f ca="1">Q19-S19</f>
         <v>4</v>
       </c>
-      <c r="V19" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W19" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>228</v>
       </c>
-      <c r="W19" s="8">
+      <c r="X19" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.86692015209125473</v>
       </c>
-      <c r="X19" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y19" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>212</v>
       </c>
-      <c r="Y19" s="8">
+      <c r="Z19" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.80608365019011408</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="49">
+      <c r="B20" s="29">
         <v>238</v>
       </c>
       <c r="E20" s="13"/>
@@ -5827,7 +5899,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="15">
-        <f t="shared" ref="K20:K37" si="16">K19+7</f>
+        <f t="shared" ref="K20:K37" si="17">K19+7</f>
         <v>43661</v>
       </c>
       <c r="L20" s="3">
@@ -5862,39 +5934,43 @@
         <v>2</v>
       </c>
       <c r="T20" s="3">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>4</v>
       </c>
       <c r="U20" s="3">
-        <f t="shared" ref="U20:U28" ca="1" si="17">Q20-S20</f>
+        <v>2</v>
+      </c>
+      <c r="V20" s="3">
+        <f t="shared" ref="V20:V28" ca="1" si="18">Q20-S20</f>
         <v>3</v>
       </c>
-      <c r="V20" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W20" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>231</v>
       </c>
-      <c r="W20" s="8">
+      <c r="X20" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.87832699619771859</v>
       </c>
-      <c r="X20" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y20" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>215</v>
       </c>
-      <c r="Y20" s="8">
+      <c r="Z20" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.81749049429657794</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="49"/>
+      <c r="B21" s="29"/>
       <c r="E21" s="8"/>
       <c r="G21" s="15"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43668</v>
       </c>
       <c r="L21" s="3">
@@ -5929,41 +6005,45 @@
         <v>3</v>
       </c>
       <c r="T21" s="3">
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="U21" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>2</v>
-      </c>
-      <c r="V21" s="16">
-        <f t="shared" ca="1" si="11"/>
+        <v>3</v>
+      </c>
+      <c r="V21" s="3">
+        <f t="shared" ca="1" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="W21" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>233</v>
       </c>
-      <c r="W21" s="8">
+      <c r="X21" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.88593155893536124</v>
       </c>
-      <c r="X21" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y21" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>217</v>
       </c>
-      <c r="Y21" s="8">
+      <c r="Z21" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.82509505703422048</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="52"/>
       <c r="E22" s="8"/>
       <c r="G22" s="15"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43675</v>
       </c>
       <c r="L22" s="3">
@@ -5998,34 +6078,38 @@
         <v>2</v>
       </c>
       <c r="T22" s="3">
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="U22" s="3">
-        <f t="shared" ca="1" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="V22" s="3">
+        <f t="shared" ca="1" si="18"/>
         <v>3</v>
       </c>
-      <c r="V22" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W22" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>236</v>
       </c>
-      <c r="W22" s="8">
+      <c r="X22" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.89733840304182511</v>
       </c>
-      <c r="X22" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y22" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>220</v>
       </c>
-      <c r="Y22" s="8">
+      <c r="Z22" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.83650190114068446</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="49">
+      <c r="B23" s="29">
         <f ca="1">SUM(Q4:INDIRECT("Q"&amp;E9))</f>
         <v>105</v>
       </c>
@@ -6035,7 +6119,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43682</v>
       </c>
       <c r="L23" s="3">
@@ -6070,34 +6154,38 @@
         <v>4</v>
       </c>
       <c r="T23" s="3">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="U23" s="3">
         <v>4</v>
       </c>
-      <c r="U23" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="V23" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V23" s="3">
+        <f t="shared" ca="1" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="W23" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>237</v>
       </c>
-      <c r="W23" s="8">
+      <c r="X23" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.90114068441064643</v>
       </c>
-      <c r="X23" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y23" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>221</v>
       </c>
-      <c r="Y23" s="8">
+      <c r="Z23" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.84030418250950567</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="49">
+      <c r="B24" s="29">
         <f ca="1">SUM(S4:INDIRECT("S"&amp;E9))</f>
         <v>31</v>
       </c>
@@ -6107,7 +6195,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43689</v>
       </c>
       <c r="L24" s="3">
@@ -6142,43 +6230,47 @@
         <v>5</v>
       </c>
       <c r="T24" s="3">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="U24" s="3">
         <v>3</v>
       </c>
-      <c r="U24" s="3">
-        <f t="shared" ca="1" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="V24" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V24" s="3">
+        <f t="shared" ca="1" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="W24" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>237</v>
       </c>
-      <c r="W24" s="8">
+      <c r="X24" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.90114068441064643</v>
       </c>
-      <c r="X24" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y24" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>221</v>
       </c>
-      <c r="Y24" s="8">
+      <c r="Z24" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.84030418250950567</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="54">
+      <c r="B25" s="34">
         <f ca="1">INDIRECT("Y"&amp;E9)</f>
-        <v>0.84030418250950567</v>
+        <v>221</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43696</v>
       </c>
       <c r="L25" s="3">
@@ -6213,43 +6305,47 @@
         <v>2</v>
       </c>
       <c r="T25" s="3">
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="U25" s="3">
-        <f t="shared" ca="1" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="V25" s="3">
+        <f t="shared" ca="1" si="18"/>
         <v>3</v>
       </c>
-      <c r="V25" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W25" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>240</v>
       </c>
-      <c r="W25" s="8">
+      <c r="X25" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.9125475285171103</v>
       </c>
-      <c r="X25" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y25" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>224</v>
       </c>
-      <c r="Y25" s="8">
+      <c r="Z25" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.85171102661596954</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="55">
+      <c r="B26" s="35">
         <f ca="1">INDIRECT("X"&amp;E9)</f>
-        <v>221</v>
+        <v>0.90114068441064643</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43703</v>
       </c>
       <c r="L26" s="3">
@@ -6284,34 +6380,38 @@
         <v>2</v>
       </c>
       <c r="T26" s="3">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="U26" s="3">
-        <f t="shared" ca="1" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="V26" s="3">
+        <f t="shared" ca="1" si="18"/>
         <v>3</v>
       </c>
-      <c r="V26" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W26" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>243</v>
       </c>
-      <c r="W26" s="8">
+      <c r="X26" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.92395437262357416</v>
       </c>
-      <c r="X26" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y26" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>227</v>
       </c>
-      <c r="Y26" s="8">
+      <c r="Z26" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.86311787072243351</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="49">
+      <c r="B27" s="29">
         <f>$E$3</f>
         <v>263</v>
       </c>
@@ -6320,7 +6420,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43710</v>
       </c>
       <c r="L27" s="3">
@@ -6355,38 +6455,42 @@
         <v>2</v>
       </c>
       <c r="T27" s="3">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>5</v>
       </c>
       <c r="U27" s="3">
-        <f t="shared" ca="1" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="V27" s="3">
+        <f t="shared" ca="1" si="18"/>
         <v>3</v>
       </c>
-      <c r="V27" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W27" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>246</v>
       </c>
-      <c r="W27" s="8">
+      <c r="X27" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.93536121673003803</v>
       </c>
-      <c r="X27" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y27" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>230</v>
       </c>
-      <c r="Y27" s="8">
+      <c r="Z27" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.87452471482889738</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="49"/>
+      <c r="B28" s="29"/>
       <c r="G28" s="15"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43717</v>
       </c>
       <c r="L28" s="3">
@@ -6421,40 +6525,44 @@
         <v>2</v>
       </c>
       <c r="T28" s="3">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>1</v>
       </c>
       <c r="U28" s="3">
-        <f t="shared" ca="1" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="V28" s="3">
+        <f t="shared" ca="1" si="18"/>
         <v>3</v>
       </c>
-      <c r="V28" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W28" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>249</v>
       </c>
-      <c r="W28" s="8">
+      <c r="X28" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.94676806083650189</v>
       </c>
-      <c r="X28" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y28" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>233</v>
       </c>
-      <c r="Y28" s="8">
+      <c r="Z28" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.88593155893536124</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A29" s="36" t="s">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="37"/>
+      <c r="B29" s="54"/>
       <c r="G29" s="15"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43724</v>
       </c>
       <c r="L29" s="3">
@@ -6489,34 +6597,38 @@
         <v>1</v>
       </c>
       <c r="T29" s="3">
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="U29" s="3">
+        <v>1</v>
+      </c>
+      <c r="V29" s="3">
         <f ca="1">Q29-S29</f>
         <v>4</v>
       </c>
-      <c r="V29" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W29" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>253</v>
       </c>
-      <c r="W29" s="8">
+      <c r="X29" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.96197718631178708</v>
       </c>
-      <c r="X29" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y29" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>237</v>
       </c>
-      <c r="Y29" s="8">
+      <c r="Z29" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.90114068441064643</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="55">
+      <c r="B30" s="35">
         <f ca="1">SUM(L4:INDIRECT("L"&amp;E9))</f>
         <v>8400</v>
       </c>
@@ -6525,7 +6637,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43731</v>
       </c>
       <c r="L30" s="3">
@@ -6560,34 +6672,38 @@
         <v>5</v>
       </c>
       <c r="T30" s="3">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="U30" s="3">
         <v>5</v>
       </c>
-      <c r="U30" s="3">
-        <f t="shared" ref="U30:U37" ca="1" si="18">Q30-S30</f>
-        <v>0</v>
-      </c>
-      <c r="V30" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V30" s="3">
+        <f t="shared" ref="V30:V37" ca="1" si="19">Q30-S30</f>
+        <v>0</v>
+      </c>
+      <c r="W30" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>253</v>
       </c>
-      <c r="W30" s="8">
+      <c r="X30" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.96197718631178708</v>
       </c>
-      <c r="X30" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y30" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>237</v>
       </c>
-      <c r="Y30" s="8">
+      <c r="Z30" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.90114068441064643</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="56">
+      <c r="B31" s="36">
         <f ca="1">B56/B30</f>
         <v>0.47619047619047616</v>
       </c>
@@ -6596,7 +6712,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43738</v>
       </c>
       <c r="L31" s="3">
@@ -6631,34 +6747,38 @@
         <v>2</v>
       </c>
       <c r="T31" s="3">
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="U31" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="V31" s="3">
+        <f t="shared" ca="1" si="19"/>
         <v>3</v>
       </c>
-      <c r="V31" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W31" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>256</v>
       </c>
-      <c r="W31" s="8">
+      <c r="X31" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.97338403041825095</v>
       </c>
-      <c r="X31" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y31" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>240</v>
       </c>
-      <c r="Y31" s="8">
+      <c r="Z31" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.9125475285171103</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="51">
+      <c r="B32" s="31">
         <f ca="1">B34/B30</f>
         <v>0.14249999999999999</v>
       </c>
@@ -6667,7 +6787,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43745</v>
       </c>
       <c r="L32" s="3">
@@ -6702,34 +6822,38 @@
         <v>2</v>
       </c>
       <c r="T32" s="3">
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
       <c r="U32" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="V32" s="3">
+        <f t="shared" ca="1" si="19"/>
         <v>3</v>
       </c>
-      <c r="V32" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W32" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>259</v>
       </c>
-      <c r="W32" s="8">
+      <c r="X32" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.98479087452471481</v>
       </c>
-      <c r="X32" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y32" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>243</v>
       </c>
-      <c r="Y32" s="8">
+      <c r="Z32" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.92395437262357416</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="49">
+      <c r="B33" s="29">
         <f ca="1">(B30/$E$10)*4</f>
         <v>1600</v>
       </c>
@@ -6738,7 +6862,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43752</v>
       </c>
       <c r="L33" s="3">
@@ -6773,34 +6897,38 @@
         <v>3</v>
       </c>
       <c r="T33" s="3">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="U33" s="3">
         <v>3</v>
       </c>
-      <c r="U33" s="3">
-        <f t="shared" ca="1" si="18"/>
-        <v>2</v>
-      </c>
-      <c r="V33" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V33" s="3">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="W33" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>261</v>
       </c>
-      <c r="W33" s="8">
+      <c r="X33" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.99239543726235746</v>
       </c>
-      <c r="X33" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y33" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>245</v>
       </c>
-      <c r="Y33" s="8">
+      <c r="Z33" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.9315589353612167</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="55">
+      <c r="B34" s="35">
         <f ca="1">SUM(M4:INDIRECT("M"&amp;E9))</f>
         <v>1197</v>
       </c>
@@ -6809,7 +6937,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43759</v>
       </c>
       <c r="L34" s="3">
@@ -6844,34 +6972,38 @@
         <v>2</v>
       </c>
       <c r="T34" s="3">
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="U34" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="V34" s="3">
+        <f t="shared" ca="1" si="19"/>
         <v>3</v>
       </c>
-      <c r="V34" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W34" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>264</v>
       </c>
-      <c r="W34" s="8">
+      <c r="X34" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0038022813688212</v>
       </c>
-      <c r="X34" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y34" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>248</v>
       </c>
-      <c r="Y34" s="8">
+      <c r="Z34" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.94296577946768056</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="56">
+      <c r="B35" s="36">
         <f ca="1">B56/B34</f>
         <v>3.3416875522138678</v>
       </c>
@@ -6880,7 +7012,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43766</v>
       </c>
       <c r="L35" s="3">
@@ -6915,34 +7047,38 @@
         <v>3</v>
       </c>
       <c r="T35" s="3">
-        <v>2</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="U35" s="3">
-        <f t="shared" ca="1" si="18"/>
-        <v>2</v>
-      </c>
-      <c r="V35" s="16">
-        <f t="shared" ca="1" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="V35" s="3">
+        <f t="shared" ca="1" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="W35" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>266</v>
       </c>
-      <c r="W35" s="8">
+      <c r="X35" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0114068441064639</v>
       </c>
-      <c r="X35" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y35" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>250</v>
       </c>
-      <c r="Y35" s="8">
+      <c r="Z35" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.95057034220532322</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="51">
+      <c r="B36" s="31">
         <f ca="1">B38/B34</f>
         <v>0.31578947368421051</v>
       </c>
@@ -6951,7 +7087,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43773</v>
       </c>
       <c r="L36" s="3">
@@ -6986,34 +7122,38 @@
         <v>4</v>
       </c>
       <c r="T36" s="3">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="U36" s="3">
         <v>4</v>
       </c>
-      <c r="U36" s="3">
-        <f t="shared" ca="1" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="V36" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="V36" s="3">
+        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="W36" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>267</v>
       </c>
-      <c r="W36" s="8">
+      <c r="X36" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0152091254752851</v>
       </c>
-      <c r="X36" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y36" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>251</v>
       </c>
-      <c r="Y36" s="8">
+      <c r="Z36" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.95437262357414454</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="49">
+      <c r="B37" s="29">
         <f ca="1">(B34/$E$10)*4</f>
         <v>228</v>
       </c>
@@ -7022,7 +7162,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="15">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>43780</v>
       </c>
       <c r="L37" s="3">
@@ -7057,44 +7197,48 @@
         <v>2</v>
       </c>
       <c r="T37" s="3">
-        <v>1</v>
+        <f>U40</f>
+        <v>0</v>
       </c>
       <c r="U37" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="V37" s="3">
+        <f t="shared" ca="1" si="19"/>
         <v>3</v>
       </c>
-      <c r="V37" s="16">
-        <f t="shared" ca="1" si="11"/>
+      <c r="W37" s="16">
+        <f t="shared" ca="1" si="12"/>
         <v>270</v>
       </c>
-      <c r="W37" s="8">
+      <c r="X37" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0266159695817489</v>
       </c>
-      <c r="X37" s="3">
-        <f t="shared" ca="1" si="12"/>
+      <c r="Y37" s="3">
+        <f t="shared" ca="1" si="13"/>
         <v>254</v>
       </c>
-      <c r="Y37" s="8">
+      <c r="Z37" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.96577946768060841</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="55">
+      <c r="B38" s="35">
         <f ca="1">SUM(N4:INDIRECT("N"&amp;E9))</f>
         <v>378</v>
       </c>
-      <c r="W38" s="8"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X38" s="8"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="56">
+      <c r="B39" s="36">
         <f ca="1">B56/B38</f>
         <v>10.582010582010582</v>
       </c>
@@ -7110,83 +7254,83 @@
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="51">
+      <c r="B40" s="31">
         <f ca="1">B42/B38</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="49">
+      <c r="B41" s="29">
         <f ca="1">(B38/E10)*4</f>
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B42" s="55">
+      <c r="B42" s="35">
         <f ca="1">SUM(O4:INDIRECT("O"&amp;E9))</f>
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="56">
+      <c r="B43" s="36">
         <f ca="1">B56/B42</f>
         <v>31.746031746031747</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="51">
+      <c r="B44" s="31">
         <f ca="1">B46/B42</f>
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="49">
+      <c r="B45" s="29">
         <f ca="1">(B42/E10)*4</f>
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="55">
+      <c r="B46" s="35">
         <f ca="1">SUM(Q4:INDIRECT("Q"&amp;E9))</f>
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B47" s="56">
+      <c r="B47" s="36">
         <f ca="1">B56/B46</f>
         <v>38.095238095238095</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B48" s="57">
+      <c r="B48" s="37">
         <f ca="1">1*B32*B36*B40*B44</f>
         <v>1.2499999999999997E-2</v>
       </c>
@@ -7195,26 +7339,26 @@
       <c r="A49" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="49">
+      <c r="B49" s="29">
         <f ca="1">(B46/E10)*4</f>
         <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
-      <c r="B50" s="49"/>
+      <c r="B50" s="29"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="40" t="s">
+      <c r="A51" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="B51" s="41"/>
+      <c r="B51" s="58"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="56">
+      <c r="B52" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7222,7 +7366,7 @@
       <c r="A53" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="56">
+      <c r="B53" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7230,7 +7374,7 @@
       <c r="A54" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="56">
+      <c r="B54" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7238,7 +7382,7 @@
       <c r="A55" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B55" s="56">
+      <c r="B55" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7246,7 +7390,7 @@
       <c r="A56" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B56" s="56">
+      <c r="B56" s="36">
         <f>SUM(B52:B55)</f>
         <v>4000</v>
       </c>
@@ -7255,7 +7399,7 @@
       <c r="A57" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="49">
+      <c r="B57" s="29">
         <f ca="1">ROUND(B58/B56,0)</f>
         <v>315</v>
       </c>
@@ -7264,26 +7408,26 @@
       <c r="A58" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B58" s="56">
+      <c r="B58" s="36">
         <f ca="1">B23*(B8*12)</f>
         <v>1260000</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
-      <c r="B59" s="56"/>
+      <c r="B59" s="36"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="42" t="s">
+      <c r="A60" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="B60" s="43"/>
+      <c r="B60" s="60"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B61" s="56">
+      <c r="B61" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7291,7 +7435,7 @@
       <c r="A62" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B62" s="56">
+      <c r="B62" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7299,7 +7443,7 @@
       <c r="A63" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B63" s="56">
+      <c r="B63" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7307,7 +7451,7 @@
       <c r="A64" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B64" s="56">
+      <c r="B64" s="36">
         <v>1000</v>
       </c>
     </row>
@@ -7315,7 +7459,7 @@
       <c r="A65" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="56">
+      <c r="B65" s="36">
         <f>SUM(B61:B64)</f>
         <v>4000</v>
       </c>
@@ -7324,35 +7468,35 @@
       <c r="A66" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B66" s="49">
+      <c r="B66" s="29">
         <f ca="1">ROUND(B67/B65,0)</f>
-        <v>174</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B67" s="56">
+      <c r="B67" s="36">
         <f ca="1">B15*(B8*12)</f>
-        <v>696000</v>
+        <v>1092000</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="56"/>
+      <c r="B68" s="36"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="26" t="s">
+      <c r="A69" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="B69" s="27"/>
+      <c r="B69" s="44"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="56">
+      <c r="B70" s="36">
         <f>B65+B56</f>
         <v>8000</v>
       </c>
@@ -7361,18 +7505,18 @@
       <c r="A71" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B71" s="49">
+      <c r="B71" s="29">
         <f ca="1">ROUND(B72/B70,0)</f>
-        <v>245</v>
+        <v>294</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B72" s="58">
+      <c r="B72" s="38">
         <f ca="1">B67+B58</f>
-        <v>1956000</v>
+        <v>2352000</v>
       </c>
     </row>
   </sheetData>
@@ -7380,7 +7524,7 @@
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="K1:Z1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A22:B22"/>

</xml_diff>

<commit_message>
updated run rate template
</commit_message>
<xml_diff>
--- a/xls/templates/run-rate-template.xlsx
+++ b/xls/templates/run-rate-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toddcullen/Projects/remarkably/xls/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DE20C7-AF93-FA4F-92B1-F912DE251932}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9875FA-F8C6-C942-A955-70D199D4807A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="1" xr2:uid="{37D2F886-AD7C-B54B-8546-6E8B72F70745}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="118">
   <si>
     <t>Start Date</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>Notice to Renew</t>
+  </si>
+  <si>
+    <t>Note - Place Acquisitioin by period up above</t>
   </si>
 </sst>
 </file>
@@ -1115,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85182B8-1FF3-A545-8EEF-BDB4651EA58C}">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4437,10 +4440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE4156A3-96B9-DE41-91DB-F4C9577E214C}">
-  <dimension ref="A1:Z72"/>
+  <dimension ref="A1:AA72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4453,17 +4456,18 @@
     <col min="13" max="13" width="6.83203125" customWidth="1"/>
     <col min="16" max="16" width="7.5" customWidth="1"/>
     <col min="17" max="17" width="6.6640625" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" customWidth="1"/>
-    <col min="19" max="19" width="9.83203125" customWidth="1"/>
-    <col min="20" max="20" width="14" customWidth="1"/>
-    <col min="21" max="21" width="9.5" customWidth="1"/>
-    <col min="22" max="22" width="22" customWidth="1"/>
-    <col min="23" max="23" width="15.33203125" customWidth="1"/>
-    <col min="25" max="25" width="14.5" customWidth="1"/>
-    <col min="26" max="26" width="16" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
+    <col min="22" max="22" width="9.5" customWidth="1"/>
+    <col min="23" max="23" width="22" customWidth="1"/>
+    <col min="24" max="24" width="15.33203125" customWidth="1"/>
+    <col min="26" max="26" width="14.5" customWidth="1"/>
+    <col min="27" max="27" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>82</v>
       </c>
@@ -4495,8 +4499,9 @@
       <c r="X1" s="48"/>
       <c r="Y1" s="48"/>
       <c r="Z1" s="48"/>
-    </row>
-    <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA1" s="48"/>
+    </row>
+    <row r="2" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="29"/>
       <c r="D2" t="s">
@@ -4534,34 +4539,37 @@
         <v>64</v>
       </c>
       <c r="R2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="U2" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="V2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="W2" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="X2" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="Y2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Z2" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="AA2" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>61</v>
       </c>
@@ -4585,24 +4593,24 @@
       <c r="K3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <f>$E$4</f>
         <v>163</v>
       </c>
-      <c r="X3" s="8">
-        <f>W3/$E$3</f>
+      <c r="Y3" s="8">
+        <f>X3/$E$3</f>
         <v>0.61977186311787069</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <f>$E$8</f>
         <v>147</v>
       </c>
-      <c r="Z3" s="8">
-        <f>Y3/$E$3</f>
+      <c r="AA3" s="8">
+        <f>Z3/$E$3</f>
         <v>0.55893536121673004</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>59</v>
       </c>
@@ -4655,41 +4663,44 @@
         <v>5</v>
       </c>
       <c r="R4" s="3">
-        <f>S7</f>
         <v>0</v>
       </c>
       <c r="S4" s="3">
+        <f>T7</f>
         <v>0</v>
       </c>
       <c r="T4" s="3">
-        <f>U7</f>
         <v>0</v>
       </c>
       <c r="U4" s="3">
+        <f>V7</f>
         <v>0</v>
       </c>
       <c r="V4" s="3">
-        <f ca="1">Q4-S4</f>
-        <v>5</v>
-      </c>
-      <c r="W4" s="16">
-        <f ca="1">W3+V4</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <f ca="1">Q4-T4</f>
+        <v>5</v>
+      </c>
+      <c r="X4" s="16">
+        <f ca="1">X3+W4</f>
         <v>168</v>
       </c>
-      <c r="X4" s="8">
-        <f t="shared" ref="X4:X37" ca="1" si="1">W4/$E$3</f>
+      <c r="Y4" s="8">
+        <f t="shared" ref="Y4:Y37" ca="1" si="1">X4/$E$3</f>
         <v>0.63878326996197721</v>
       </c>
-      <c r="Y4" s="3">
-        <f ca="1">Y3+Q4-S4</f>
+      <c r="Z4" s="3">
+        <f ca="1">Z3+Q4-T4</f>
         <v>152</v>
       </c>
-      <c r="Z4" s="8">
-        <f t="shared" ref="Z4:Z37" ca="1" si="2">Y4/$E$3</f>
+      <c r="AA4" s="8">
+        <f t="shared" ref="AA4:AA37" ca="1" si="2">Z4/$E$3</f>
         <v>0.57794676806083645</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -4742,41 +4753,44 @@
         <v>5</v>
       </c>
       <c r="R5" s="3">
-        <f t="shared" ref="R5:R37" si="9">S8</f>
         <v>0</v>
       </c>
       <c r="S5" s="3">
+        <f t="shared" ref="S5:S37" si="9">T8</f>
         <v>0</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" ref="T5:T36" si="10">U8</f>
         <v>0</v>
       </c>
       <c r="U5" s="3">
+        <f t="shared" ref="U5:U36" si="10">V8</f>
         <v>0</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" ref="V5:V13" ca="1" si="11">Q5-S5</f>
-        <v>5</v>
-      </c>
-      <c r="W5" s="16">
-        <f t="shared" ref="W5:W37" ca="1" si="12">W4+V5</f>
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <f ca="1">Q5-T5</f>
+        <v>5</v>
+      </c>
+      <c r="X5" s="16">
+        <f t="shared" ref="X5:X37" ca="1" si="11">X4+W5</f>
         <v>173</v>
       </c>
-      <c r="X5" s="8">
+      <c r="Y5" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.65779467680608361</v>
       </c>
-      <c r="Y5" s="3">
-        <f t="shared" ref="Y5:Y37" ca="1" si="13">Y4+Q5-S5</f>
+      <c r="Z5" s="3">
+        <f ca="1">Z4+Q5-T5</f>
         <v>157</v>
       </c>
-      <c r="Z5" s="8">
+      <c r="AA5" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.59695817490494296</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
@@ -4803,7 +4817,7 @@
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="15">
-        <f t="shared" ref="K6:K11" si="14">K5+7</f>
+        <f t="shared" ref="K6:K11" si="12">K5+7</f>
         <v>43563</v>
       </c>
       <c r="L6" s="3">
@@ -4831,41 +4845,44 @@
         <v>5</v>
       </c>
       <c r="R6" s="3">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
       <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
       <c r="V6" s="3">
+        <v>0</v>
+      </c>
+      <c r="W6" s="3">
+        <f ca="1">Q6-T6</f>
+        <v>5</v>
+      </c>
+      <c r="X6" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="W6" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>178</v>
       </c>
-      <c r="X6" s="8">
+      <c r="Y6" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.67680608365019013</v>
       </c>
-      <c r="Y6" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z6" s="3">
+        <f ca="1">Z5+Q6-T6</f>
         <v>162</v>
       </c>
-      <c r="Z6" s="8">
+      <c r="AA6" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.61596958174904948</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
@@ -4892,7 +4909,7 @@
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>43570</v>
       </c>
       <c r="L7" s="3">
@@ -4920,41 +4937,45 @@
         <v>5</v>
       </c>
       <c r="R7" s="3">
+        <f ca="1">Q4</f>
+        <v>5</v>
+      </c>
+      <c r="S7" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S7" s="3">
-        <v>0</v>
-      </c>
       <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U7" s="3">
-        <v>0</v>
-      </c>
       <c r="V7" s="3">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3">
+        <f ca="1">Q7-T7</f>
+        <v>5</v>
+      </c>
+      <c r="X7" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="W7" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>183</v>
       </c>
-      <c r="X7" s="8">
+      <c r="Y7" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.69581749049429653</v>
       </c>
-      <c r="Y7" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z7" s="3">
+        <f ca="1">Z6+Q7-T7</f>
         <v>167</v>
       </c>
-      <c r="Z7" s="8">
+      <c r="AA7" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.63498098859315588</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -4973,7 +4994,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>43577</v>
       </c>
       <c r="L8" s="3">
@@ -5001,41 +5022,45 @@
         <v>5</v>
       </c>
       <c r="R8" s="3">
+        <f t="shared" ref="R8:R37" ca="1" si="13">Q5</f>
+        <v>5</v>
+      </c>
+      <c r="S8" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S8" s="3">
-        <v>0</v>
-      </c>
       <c r="T8" s="3">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U8" s="3">
-        <v>0</v>
-      </c>
       <c r="V8" s="3">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
+        <f ca="1">Q8-T8</f>
+        <v>5</v>
+      </c>
+      <c r="X8" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="W8" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>188</v>
       </c>
-      <c r="X8" s="8">
+      <c r="Y8" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.71482889733840305</v>
       </c>
-      <c r="Y8" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z8" s="3">
+        <f ca="1">Z7+Q8-T8</f>
         <v>172</v>
       </c>
-      <c r="Z8" s="8">
+      <c r="AA8" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.6539923954372624</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="33"/>
       <c r="D9" t="s">
@@ -5049,7 +5074,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>43584</v>
       </c>
       <c r="L9" s="3">
@@ -5077,41 +5102,45 @@
         <v>5</v>
       </c>
       <c r="R9" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S9" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S9" s="3">
-        <v>0</v>
-      </c>
       <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U9" s="3">
-        <v>0</v>
-      </c>
       <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <f ca="1">Q9-T9</f>
+        <v>5</v>
+      </c>
+      <c r="X9" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="W9" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>193</v>
       </c>
-      <c r="X9" s="8">
+      <c r="Y9" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.73384030418250945</v>
       </c>
-      <c r="Y9" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z9" s="3">
+        <f ca="1">Z8+Q9-T9</f>
         <v>177</v>
       </c>
-      <c r="Z9" s="8">
+      <c r="AA9" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.6730038022813688</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="49" t="s">
         <v>4</v>
       </c>
@@ -5128,7 +5157,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>43591</v>
       </c>
       <c r="L10" s="3">
@@ -5156,47 +5185,51 @@
         <v>5</v>
       </c>
       <c r="R10" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S10" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S10" s="3">
-        <v>0</v>
-      </c>
       <c r="T10" s="3">
+        <v>0</v>
+      </c>
+      <c r="U10" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U10" s="3">
-        <v>0</v>
-      </c>
       <c r="V10" s="3">
+        <v>0</v>
+      </c>
+      <c r="W10" s="3">
+        <f ca="1">Q10-T10</f>
+        <v>5</v>
+      </c>
+      <c r="X10" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="W10" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>198</v>
       </c>
-      <c r="X10" s="8">
+      <c r="Y10" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.75285171102661597</v>
       </c>
-      <c r="Y10" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z10" s="3">
+        <f ca="1">Z9+Q10-T10</f>
         <v>182</v>
       </c>
-      <c r="Z10" s="8">
+      <c r="AA10" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.69201520912547532</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="29">
-        <f ca="1">INDIRECT("V"&amp;E9)-W3</f>
-        <v>-163</v>
+        <f ca="1">INDIRECT("V"&amp;E9)-X3</f>
+        <v>-160</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
@@ -5209,7 +5242,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>43598</v>
       </c>
       <c r="L11" s="3">
@@ -5237,41 +5270,45 @@
         <v>5</v>
       </c>
       <c r="R11" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S11" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S11" s="3">
-        <v>0</v>
-      </c>
       <c r="T11" s="3">
+        <v>0</v>
+      </c>
+      <c r="U11" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U11" s="3">
-        <v>0</v>
-      </c>
       <c r="V11" s="3">
+        <v>0</v>
+      </c>
+      <c r="W11" s="3">
+        <f ca="1">Q11-T11</f>
+        <v>5</v>
+      </c>
+      <c r="X11" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>5</v>
-      </c>
-      <c r="W11" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>203</v>
       </c>
-      <c r="X11" s="8">
+      <c r="Y11" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.77186311787072248</v>
       </c>
-      <c r="Y11" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z11" s="3">
+        <f ca="1">Z10+Q11-T11</f>
         <v>187</v>
       </c>
-      <c r="Z11" s="8">
+      <c r="AA11" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.71102661596958172</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
@@ -5318,41 +5355,45 @@
         <v>5</v>
       </c>
       <c r="R12" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S12" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S12" s="3">
-        <v>2</v>
-      </c>
       <c r="T12" s="3">
+        <v>2</v>
+      </c>
+      <c r="U12" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U12" s="3">
-        <v>2</v>
-      </c>
       <c r="V12" s="3">
+        <v>2</v>
+      </c>
+      <c r="W12" s="3">
+        <f ca="1">Q12-T12</f>
+        <v>3</v>
+      </c>
+      <c r="X12" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="W12" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>206</v>
       </c>
-      <c r="X12" s="8">
+      <c r="Y12" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.78326996197718635</v>
       </c>
-      <c r="Y12" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z12" s="3">
+        <f ca="1">Z11+Q12-T12</f>
         <v>190</v>
       </c>
-      <c r="Z12" s="8">
+      <c r="AA12" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.72243346007604559</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -5394,54 +5435,58 @@
         <v>5</v>
       </c>
       <c r="R13" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S13" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S13" s="3">
-        <v>2</v>
-      </c>
       <c r="T13" s="3">
+        <v>2</v>
+      </c>
+      <c r="U13" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U13" s="3">
-        <v>2</v>
-      </c>
       <c r="V13" s="3">
+        <v>2</v>
+      </c>
+      <c r="W13" s="3">
+        <f ca="1">Q13-T13</f>
+        <v>3</v>
+      </c>
+      <c r="X13" s="16">
         <f t="shared" ca="1" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="W13" s="16">
-        <f t="shared" ca="1" si="12"/>
         <v>209</v>
       </c>
-      <c r="X13" s="8">
+      <c r="Y13" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.79467680608365021</v>
       </c>
-      <c r="Y13" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z13" s="3">
+        <f ca="1">Z12+Q13-T13</f>
         <v>193</v>
       </c>
-      <c r="Z13" s="8">
+      <c r="AA13" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.73384030418250945</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="29">
-        <f ca="1">SUM(U4:INDIRECT("S"&amp;E9))</f>
-        <v>91</v>
+        <f ca="1">SUM(V4:INDIRECT("S"&amp;E9))</f>
+        <v>128</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="15">
-        <f t="shared" ref="K14:K18" si="15">K13+7</f>
+        <f t="shared" ref="K14:K18" si="14">K13+7</f>
         <v>43619</v>
       </c>
       <c r="L14" s="3">
@@ -5469,47 +5514,51 @@
         <v>5</v>
       </c>
       <c r="R14" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S14" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S14" s="3">
-        <v>2</v>
-      </c>
       <c r="T14" s="3">
+        <v>2</v>
+      </c>
+      <c r="U14" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U14" s="3">
-        <v>2</v>
-      </c>
       <c r="V14" s="3">
-        <f ca="1">Q14-S14</f>
+        <v>2</v>
+      </c>
+      <c r="W14" s="3">
+        <f ca="1">Q14-T14</f>
         <v>3</v>
       </c>
-      <c r="W14" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X14" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>212</v>
       </c>
-      <c r="X14" s="8">
+      <c r="Y14" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.80608365019011408</v>
       </c>
-      <c r="Y14" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z14" s="3">
+        <f ca="1">Z13+Q14-T14</f>
         <v>196</v>
       </c>
-      <c r="Z14" s="8">
+      <c r="AA14" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.74524714828897343</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="29">
         <f ca="1">B14</f>
-        <v>91</v>
+        <v>128</v>
       </c>
       <c r="D15" t="s">
         <v>112</v>
@@ -5519,7 +5568,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>43626</v>
       </c>
       <c r="L15" s="3">
@@ -5547,47 +5596,51 @@
         <v>5</v>
       </c>
       <c r="R15" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S15" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S15" s="3">
-        <v>2</v>
-      </c>
       <c r="T15" s="3">
+        <v>2</v>
+      </c>
+      <c r="U15" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U15" s="3">
-        <v>2</v>
-      </c>
       <c r="V15" s="3">
-        <f t="shared" ref="V15:V18" ca="1" si="16">Q15-S15</f>
+        <v>2</v>
+      </c>
+      <c r="W15" s="3">
+        <f ca="1">Q15-T15</f>
         <v>3</v>
       </c>
-      <c r="W15" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X15" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>215</v>
       </c>
-      <c r="X15" s="8">
+      <c r="Y15" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.81749049429657794</v>
       </c>
-      <c r="Y15" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z15" s="3">
+        <f ca="1">Z14+Q15-T15</f>
         <v>199</v>
       </c>
-      <c r="Z15" s="8">
+      <c r="AA15" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.75665399239543729</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="31">
         <f ca="1">B15/B17</f>
-        <v>0.7109375</v>
+        <v>0.50196078431372548</v>
       </c>
       <c r="D16" t="s">
         <v>113</v>
@@ -5597,7 +5650,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>43633</v>
       </c>
       <c r="L16" s="3">
@@ -5625,47 +5678,51 @@
         <v>5</v>
       </c>
       <c r="R16" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S16" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="S16" s="3">
-        <v>2</v>
-      </c>
       <c r="T16" s="3">
+        <v>2</v>
+      </c>
+      <c r="U16" s="3">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="U16" s="3">
-        <v>0</v>
-      </c>
       <c r="V16" s="3">
-        <f t="shared" ca="1" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="W16" s="3">
+        <f ca="1">Q16-T16</f>
         <v>3</v>
       </c>
-      <c r="W16" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X16" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>218</v>
       </c>
-      <c r="X16" s="8">
+      <c r="Y16" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.82889733840304181</v>
       </c>
-      <c r="Y16" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z16" s="3">
+        <f ca="1">Z15+Q16-T16</f>
         <v>202</v>
       </c>
-      <c r="Z16" s="8">
+      <c r="AA16" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.76806083650190116</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="29">
         <f ca="1">B18+B15</f>
-        <v>128</v>
+        <v>255</v>
       </c>
       <c r="D17" t="s">
         <v>114</v>
@@ -5675,7 +5732,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>43640</v>
       </c>
       <c r="L17" s="3">
@@ -5703,54 +5760,58 @@
         <v>5</v>
       </c>
       <c r="R17" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S17" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S17" s="3">
-        <v>2</v>
-      </c>
       <c r="T17" s="3">
+        <v>2</v>
+      </c>
+      <c r="U17" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U17" s="3">
-        <v>2</v>
-      </c>
       <c r="V17" s="3">
-        <f t="shared" ca="1" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="W17" s="3">
+        <f ca="1">Q17-T17</f>
         <v>3</v>
       </c>
-      <c r="W17" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X17" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>221</v>
       </c>
-      <c r="X17" s="8">
+      <c r="Y17" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.84030418250950567</v>
       </c>
-      <c r="Y17" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z17" s="3">
+        <f ca="1">Z16+Q17-T17</f>
         <v>205</v>
       </c>
-      <c r="Z17" s="8">
+      <c r="AA17" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.77946768060836502</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="29">
-        <f ca="1">SUM(R4:INDIRECT("R"&amp;E9))</f>
-        <v>37</v>
+        <f ca="1">SUM(S4:INDIRECT("R"&amp;E9))</f>
+        <v>127</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="15">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>43647</v>
       </c>
       <c r="L18" s="3">
@@ -5778,41 +5839,45 @@
         <v>5</v>
       </c>
       <c r="R18" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S18" s="3">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="S18" s="3">
-        <v>2</v>
-      </c>
       <c r="T18" s="3">
+        <v>2</v>
+      </c>
+      <c r="U18" s="3">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="U18" s="3">
-        <v>2</v>
-      </c>
       <c r="V18" s="3">
-        <f t="shared" ca="1" si="16"/>
+        <v>2</v>
+      </c>
+      <c r="W18" s="3">
+        <f ca="1">Q18-T18</f>
         <v>3</v>
       </c>
-      <c r="W18" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X18" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>224</v>
       </c>
-      <c r="X18" s="8">
+      <c r="Y18" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.85171102661596954</v>
       </c>
-      <c r="Y18" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z18" s="3">
+        <f ca="1">Z17+Q18-T18</f>
         <v>208</v>
       </c>
-      <c r="Z18" s="8">
+      <c r="AA18" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.79087452471482889</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
@@ -5852,41 +5917,45 @@
         <v>5</v>
       </c>
       <c r="R19" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S19" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S19" s="3">
-        <v>1</v>
-      </c>
       <c r="T19" s="3">
+        <v>1</v>
+      </c>
+      <c r="U19" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U19" s="3">
-        <v>1</v>
-      </c>
       <c r="V19" s="3">
-        <f ca="1">Q19-S19</f>
+        <v>1</v>
+      </c>
+      <c r="W19" s="3">
+        <f ca="1">Q19-T19</f>
         <v>4</v>
       </c>
-      <c r="W19" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X19" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>228</v>
       </c>
-      <c r="X19" s="8">
+      <c r="Y19" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.86692015209125473</v>
       </c>
-      <c r="Y19" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z19" s="3">
+        <f ca="1">Z18+Q19-T19</f>
         <v>212</v>
       </c>
-      <c r="Z19" s="8">
+      <c r="AA19" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.80608365019011408</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
@@ -5899,7 +5968,7 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="15">
-        <f t="shared" ref="K20:K37" si="17">K19+7</f>
+        <f t="shared" ref="K20:K37" si="15">K19+7</f>
         <v>43661</v>
       </c>
       <c r="L20" s="3">
@@ -5927,41 +5996,45 @@
         <v>5</v>
       </c>
       <c r="R20" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S20" s="3">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="S20" s="3">
-        <v>2</v>
-      </c>
       <c r="T20" s="3">
+        <v>2</v>
+      </c>
+      <c r="U20" s="3">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="U20" s="3">
-        <v>2</v>
-      </c>
       <c r="V20" s="3">
-        <f t="shared" ref="V20:V28" ca="1" si="18">Q20-S20</f>
+        <v>2</v>
+      </c>
+      <c r="W20" s="3">
+        <f ca="1">Q20-T20</f>
         <v>3</v>
       </c>
-      <c r="W20" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X20" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>231</v>
       </c>
-      <c r="X20" s="8">
+      <c r="Y20" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.87832699619771859</v>
       </c>
-      <c r="Y20" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z20" s="3">
+        <f ca="1">Z19+Q20-T20</f>
         <v>215</v>
       </c>
-      <c r="Z20" s="8">
+      <c r="AA20" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.81749049429657794</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="29"/>
       <c r="E21" s="8"/>
@@ -5970,7 +6043,7 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43668</v>
       </c>
       <c r="L21" s="3">
@@ -5998,41 +6071,45 @@
         <v>5</v>
       </c>
       <c r="R21" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S21" s="3">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="S21" s="3">
+      <c r="T21" s="3">
         <v>3</v>
       </c>
-      <c r="T21" s="3">
+      <c r="U21" s="3">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="U21" s="3">
+      <c r="V21" s="3">
         <v>3</v>
       </c>
-      <c r="V21" s="3">
-        <f t="shared" ca="1" si="18"/>
-        <v>2</v>
-      </c>
-      <c r="W21" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="W21" s="3">
+        <f ca="1">Q21-T21</f>
+        <v>2</v>
+      </c>
+      <c r="X21" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>233</v>
       </c>
-      <c r="X21" s="8">
+      <c r="Y21" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.88593155893536124</v>
       </c>
-      <c r="Y21" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z21" s="3">
+        <f ca="1">Z20+Q21-T21</f>
         <v>217</v>
       </c>
-      <c r="Z21" s="8">
+      <c r="AA21" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.82509505703422048</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="51" t="s">
         <v>15</v>
       </c>
@@ -6043,7 +6120,7 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43675</v>
       </c>
       <c r="L22" s="3">
@@ -6071,41 +6148,45 @@
         <v>5</v>
       </c>
       <c r="R22" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S22" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S22" s="3">
-        <v>2</v>
-      </c>
       <c r="T22" s="3">
+        <v>2</v>
+      </c>
+      <c r="U22" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U22" s="3">
-        <v>2</v>
-      </c>
       <c r="V22" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="W22" s="3">
+        <f ca="1">Q22-T22</f>
         <v>3</v>
       </c>
-      <c r="W22" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X22" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>236</v>
       </c>
-      <c r="X22" s="8">
+      <c r="Y22" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.89733840304182511</v>
       </c>
-      <c r="Y22" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z22" s="3">
+        <f ca="1">Z21+Q22-T22</f>
         <v>220</v>
       </c>
-      <c r="Z22" s="8">
+      <c r="AA22" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.83650190114068446</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>16</v>
       </c>
@@ -6119,7 +6200,7 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43682</v>
       </c>
       <c r="L23" s="3">
@@ -6147,47 +6228,51 @@
         <v>5</v>
       </c>
       <c r="R23" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S23" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S23" s="3">
+      <c r="T23" s="3">
         <v>4</v>
       </c>
-      <c r="T23" s="3">
+      <c r="U23" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U23" s="3">
+      <c r="V23" s="3">
         <v>4</v>
       </c>
-      <c r="V23" s="3">
-        <f t="shared" ca="1" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="W23" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="W23" s="3">
+        <f ca="1">Q23-T23</f>
+        <v>1</v>
+      </c>
+      <c r="X23" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>237</v>
       </c>
-      <c r="X23" s="8">
+      <c r="Y23" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.90114068441064643</v>
       </c>
-      <c r="Y23" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z23" s="3">
+        <f ca="1">Z22+Q23-T23</f>
         <v>221</v>
       </c>
-      <c r="Z23" s="8">
+      <c r="AA23" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.84030418250950567</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="29">
-        <f ca="1">SUM(S4:INDIRECT("S"&amp;E9))</f>
-        <v>31</v>
+        <f ca="1">SUM(T4:INDIRECT("S"&amp;E9))</f>
+        <v>68</v>
       </c>
       <c r="E24" s="12"/>
       <c r="G24" s="15"/>
@@ -6195,7 +6280,7 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43689</v>
       </c>
       <c r="L24" s="3">
@@ -6223,54 +6308,58 @@
         <v>5</v>
       </c>
       <c r="R24" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S24" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S24" s="3">
-        <v>5</v>
-      </c>
       <c r="T24" s="3">
+        <v>5</v>
+      </c>
+      <c r="U24" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U24" s="3">
+      <c r="V24" s="3">
         <v>3</v>
       </c>
-      <c r="V24" s="3">
-        <f t="shared" ca="1" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="W24" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="W24" s="3">
+        <f ca="1">Q24-T24</f>
+        <v>0</v>
+      </c>
+      <c r="X24" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>237</v>
       </c>
-      <c r="X24" s="8">
+      <c r="Y24" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.90114068441064643</v>
       </c>
-      <c r="Y24" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z24" s="3">
+        <f ca="1">Z23+Q24-T24</f>
         <v>221</v>
       </c>
-      <c r="Z24" s="8">
+      <c r="AA24" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.84030418250950567</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="34">
         <f ca="1">INDIRECT("Y"&amp;E9)</f>
-        <v>221</v>
+        <v>0.90114068441064643</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43696</v>
       </c>
       <c r="L25" s="3">
@@ -6298,54 +6387,58 @@
         <v>5</v>
       </c>
       <c r="R25" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S25" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S25" s="3">
-        <v>2</v>
-      </c>
       <c r="T25" s="3">
+        <v>2</v>
+      </c>
+      <c r="U25" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U25" s="3">
-        <v>2</v>
-      </c>
       <c r="V25" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="W25" s="3">
+        <f ca="1">Q25-T25</f>
         <v>3</v>
       </c>
-      <c r="W25" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X25" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>240</v>
       </c>
-      <c r="X25" s="8">
+      <c r="Y25" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.9125475285171103</v>
       </c>
-      <c r="Y25" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z25" s="3">
+        <f ca="1">Z24+Q25-T25</f>
         <v>224</v>
       </c>
-      <c r="Z25" s="8">
+      <c r="AA25" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.85171102661596954</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="35">
         <f ca="1">INDIRECT("X"&amp;E9)</f>
-        <v>0.90114068441064643</v>
+        <v>237</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43703</v>
       </c>
       <c r="L26" s="3">
@@ -6373,41 +6466,45 @@
         <v>5</v>
       </c>
       <c r="R26" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S26" s="3">
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-      <c r="S26" s="3">
-        <v>2</v>
-      </c>
       <c r="T26" s="3">
+        <v>2</v>
+      </c>
+      <c r="U26" s="3">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="U26" s="3">
-        <v>2</v>
-      </c>
       <c r="V26" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="W26" s="3">
+        <f ca="1">Q26-T26</f>
         <v>3</v>
       </c>
-      <c r="W26" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X26" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>243</v>
       </c>
-      <c r="X26" s="8">
+      <c r="Y26" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.92395437262357416</v>
       </c>
-      <c r="Y26" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z26" s="3">
+        <f ca="1">Z25+Q26-T26</f>
         <v>227</v>
       </c>
-      <c r="Z26" s="8">
+      <c r="AA26" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.86311787072243351</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>20</v>
       </c>
@@ -6420,7 +6517,7 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43710</v>
       </c>
       <c r="L27" s="3">
@@ -6448,41 +6545,45 @@
         <v>5</v>
       </c>
       <c r="R27" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S27" s="3">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="S27" s="3">
-        <v>2</v>
-      </c>
       <c r="T27" s="3">
+        <v>2</v>
+      </c>
+      <c r="U27" s="3">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="U27" s="3">
-        <v>2</v>
-      </c>
       <c r="V27" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="W27" s="3">
+        <f ca="1">Q27-T27</f>
         <v>3</v>
       </c>
-      <c r="W27" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X27" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>246</v>
       </c>
-      <c r="X27" s="8">
+      <c r="Y27" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.93536121673003803</v>
       </c>
-      <c r="Y27" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z27" s="3">
+        <f ca="1">Z26+Q27-T27</f>
         <v>230</v>
       </c>
-      <c r="Z27" s="8">
+      <c r="AA27" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.87452471482889738</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="29"/>
       <c r="G28" s="15"/>
@@ -6490,7 +6591,7 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43717</v>
       </c>
       <c r="L28" s="3">
@@ -6518,41 +6619,45 @@
         <v>5</v>
       </c>
       <c r="R28" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S28" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S28" s="3">
-        <v>2</v>
-      </c>
       <c r="T28" s="3">
+        <v>2</v>
+      </c>
+      <c r="U28" s="3">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="U28" s="3">
-        <v>2</v>
-      </c>
       <c r="V28" s="3">
-        <f t="shared" ca="1" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="W28" s="3">
+        <f ca="1">Q28-T28</f>
         <v>3</v>
       </c>
-      <c r="W28" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X28" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>249</v>
       </c>
-      <c r="X28" s="8">
+      <c r="Y28" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.94676806083650189</v>
       </c>
-      <c r="Y28" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z28" s="3">
+        <f ca="1">Z27+Q28-T28</f>
         <v>233</v>
       </c>
-      <c r="Z28" s="8">
+      <c r="AA28" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.88593155893536124</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="53" t="s">
         <v>21</v>
       </c>
@@ -6562,7 +6667,7 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43724</v>
       </c>
       <c r="L29" s="3">
@@ -6590,41 +6695,45 @@
         <v>5</v>
       </c>
       <c r="R29" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S29" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S29" s="3">
-        <v>1</v>
-      </c>
       <c r="T29" s="3">
+        <v>1</v>
+      </c>
+      <c r="U29" s="3">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="U29" s="3">
-        <v>1</v>
-      </c>
       <c r="V29" s="3">
-        <f ca="1">Q29-S29</f>
+        <v>1</v>
+      </c>
+      <c r="W29" s="3">
+        <f ca="1">Q29-T29</f>
         <v>4</v>
       </c>
-      <c r="W29" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X29" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>253</v>
       </c>
-      <c r="X29" s="8">
+      <c r="Y29" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.96197718631178708</v>
       </c>
-      <c r="Y29" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z29" s="3">
+        <f ca="1">Z28+Q29-T29</f>
         <v>237</v>
       </c>
-      <c r="Z29" s="8">
+      <c r="AA29" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.90114068441064643</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>22</v>
       </c>
@@ -6637,7 +6746,7 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43731</v>
       </c>
       <c r="L30" s="3">
@@ -6665,41 +6774,45 @@
         <v>5</v>
       </c>
       <c r="R30" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S30" s="3">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="S30" s="3">
-        <v>5</v>
-      </c>
       <c r="T30" s="3">
+        <v>5</v>
+      </c>
+      <c r="U30" s="3">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="U30" s="3">
-        <v>5</v>
-      </c>
       <c r="V30" s="3">
-        <f t="shared" ref="V30:V37" ca="1" si="19">Q30-S30</f>
-        <v>0</v>
-      </c>
-      <c r="W30" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="W30" s="3">
+        <f ca="1">Q30-T30</f>
+        <v>0</v>
+      </c>
+      <c r="X30" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>253</v>
       </c>
-      <c r="X30" s="8">
+      <c r="Y30" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.96197718631178708</v>
       </c>
-      <c r="Y30" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z30" s="3">
+        <f ca="1">Z29+Q30-T30</f>
         <v>237</v>
       </c>
-      <c r="Z30" s="8">
+      <c r="AA30" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.90114068441064643</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
@@ -6712,7 +6825,7 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43738</v>
       </c>
       <c r="L31" s="3">
@@ -6740,41 +6853,45 @@
         <v>5</v>
       </c>
       <c r="R31" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S31" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S31" s="3">
-        <v>2</v>
-      </c>
       <c r="T31" s="3">
+        <v>2</v>
+      </c>
+      <c r="U31" s="3">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="U31" s="3">
-        <v>1</v>
-      </c>
       <c r="V31" s="3">
-        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="W31" s="3">
+        <f ca="1">Q31-T31</f>
         <v>3</v>
       </c>
-      <c r="W31" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X31" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>256</v>
       </c>
-      <c r="X31" s="8">
+      <c r="Y31" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.97338403041825095</v>
       </c>
-      <c r="Y31" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z31" s="3">
+        <f ca="1">Z30+Q31-T31</f>
         <v>240</v>
       </c>
-      <c r="Z31" s="8">
+      <c r="AA31" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.9125475285171103</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>24</v>
       </c>
@@ -6787,7 +6904,7 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43745</v>
       </c>
       <c r="L32" s="3">
@@ -6815,41 +6932,45 @@
         <v>5</v>
       </c>
       <c r="R32" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S32" s="3">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="S32" s="3">
-        <v>2</v>
-      </c>
       <c r="T32" s="3">
+        <v>2</v>
+      </c>
+      <c r="U32" s="3">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="U32" s="3">
-        <v>1</v>
-      </c>
       <c r="V32" s="3">
-        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="W32" s="3">
+        <f ca="1">Q32-T32</f>
         <v>3</v>
       </c>
-      <c r="W32" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X32" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>259</v>
       </c>
-      <c r="X32" s="8">
+      <c r="Y32" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.98479087452471481</v>
       </c>
-      <c r="Y32" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z32" s="3">
+        <f ca="1">Z31+Q32-T32</f>
         <v>243</v>
       </c>
-      <c r="Z32" s="8">
+      <c r="AA32" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.92395437262357416</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>25</v>
       </c>
@@ -6862,7 +6983,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43752</v>
       </c>
       <c r="L33" s="3">
@@ -6890,41 +7011,45 @@
         <v>5</v>
       </c>
       <c r="R33" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S33" s="3">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="S33" s="3">
+      <c r="T33" s="3">
         <v>3</v>
       </c>
-      <c r="T33" s="3">
+      <c r="U33" s="3">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="U33" s="3">
+      <c r="V33" s="3">
         <v>3</v>
       </c>
-      <c r="V33" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>2</v>
-      </c>
-      <c r="W33" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="W33" s="3">
+        <f ca="1">Q33-T33</f>
+        <v>2</v>
+      </c>
+      <c r="X33" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>261</v>
       </c>
-      <c r="X33" s="8">
+      <c r="Y33" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>0.99239543726235746</v>
       </c>
-      <c r="Y33" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z33" s="3">
+        <f ca="1">Z32+Q33-T33</f>
         <v>245</v>
       </c>
-      <c r="Z33" s="8">
+      <c r="AA33" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.9315589353612167</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>26</v>
       </c>
@@ -6937,7 +7062,7 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43759</v>
       </c>
       <c r="L34" s="3">
@@ -6965,41 +7090,45 @@
         <v>5</v>
       </c>
       <c r="R34" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S34" s="3">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="S34" s="3">
-        <v>2</v>
-      </c>
       <c r="T34" s="3">
+        <v>2</v>
+      </c>
+      <c r="U34" s="3">
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="U34" s="3">
-        <v>1</v>
-      </c>
       <c r="V34" s="3">
-        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="W34" s="3">
+        <f ca="1">Q34-T34</f>
         <v>3</v>
       </c>
-      <c r="W34" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X34" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>264</v>
       </c>
-      <c r="X34" s="8">
+      <c r="Y34" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0038022813688212</v>
       </c>
-      <c r="Y34" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z34" s="3">
+        <f ca="1">Z33+Q34-T34</f>
         <v>248</v>
       </c>
-      <c r="Z34" s="8">
+      <c r="AA34" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.94296577946768056</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>27</v>
       </c>
@@ -7012,7 +7141,7 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43766</v>
       </c>
       <c r="L35" s="3">
@@ -7040,41 +7169,45 @@
         <v>5</v>
       </c>
       <c r="R35" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S35" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S35" s="3">
+      <c r="T35" s="3">
         <v>3</v>
       </c>
-      <c r="T35" s="3">
+      <c r="U35" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U35" s="3">
-        <v>2</v>
-      </c>
       <c r="V35" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>2</v>
-      </c>
-      <c r="W35" s="16">
-        <f t="shared" ca="1" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="W35" s="3">
+        <f ca="1">Q35-T35</f>
+        <v>2</v>
+      </c>
+      <c r="X35" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>266</v>
       </c>
-      <c r="X35" s="8">
+      <c r="Y35" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0114068441064639</v>
       </c>
-      <c r="Y35" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z35" s="3">
+        <f ca="1">Z34+Q35-T35</f>
         <v>250</v>
       </c>
-      <c r="Z35" s="8">
+      <c r="AA35" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.95057034220532322</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>28</v>
       </c>
@@ -7087,7 +7220,7 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43773</v>
       </c>
       <c r="L36" s="3">
@@ -7115,41 +7248,45 @@
         <v>5</v>
       </c>
       <c r="R36" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S36" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S36" s="3">
+      <c r="T36" s="3">
         <v>4</v>
       </c>
-      <c r="T36" s="3">
+      <c r="U36" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="U36" s="3">
+      <c r="V36" s="3">
         <v>4</v>
       </c>
-      <c r="V36" s="3">
-        <f t="shared" ca="1" si="19"/>
-        <v>1</v>
-      </c>
-      <c r="W36" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="W36" s="3">
+        <f ca="1">Q36-T36</f>
+        <v>1</v>
+      </c>
+      <c r="X36" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>267</v>
       </c>
-      <c r="X36" s="8">
+      <c r="Y36" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0152091254752851</v>
       </c>
-      <c r="Y36" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z36" s="3">
+        <f ca="1">Z35+Q36-T36</f>
         <v>251</v>
       </c>
-      <c r="Z36" s="8">
+      <c r="AA36" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.95437262357414454</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>29</v>
       </c>
@@ -7162,7 +7299,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>43780</v>
       </c>
       <c r="L37" s="3">
@@ -7190,41 +7327,45 @@
         <v>5</v>
       </c>
       <c r="R37" s="3">
+        <f t="shared" ca="1" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="S37" s="3">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="S37" s="3">
-        <v>2</v>
-      </c>
       <c r="T37" s="3">
-        <f>U40</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U37" s="3">
-        <v>1</v>
+        <f>V40</f>
+        <v>0</v>
       </c>
       <c r="V37" s="3">
-        <f t="shared" ca="1" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="W37" s="3">
+        <f ca="1">Q37-T37</f>
         <v>3</v>
       </c>
-      <c r="W37" s="16">
-        <f t="shared" ca="1" si="12"/>
+      <c r="X37" s="16">
+        <f t="shared" ca="1" si="11"/>
         <v>270</v>
       </c>
-      <c r="X37" s="8">
+      <c r="Y37" s="8">
         <f t="shared" ca="1" si="1"/>
         <v>1.0266159695817489</v>
       </c>
-      <c r="Y37" s="3">
-        <f t="shared" ca="1" si="13"/>
+      <c r="Z37" s="3">
+        <f ca="1">Z36+Q37-T37</f>
         <v>254</v>
       </c>
-      <c r="Z37" s="8">
+      <c r="AA37" s="8">
         <f t="shared" ca="1" si="2"/>
         <v>0.96577946768060841</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>30</v>
       </c>
@@ -7232,9 +7373,10 @@
         <f ca="1">SUM(N4:INDIRECT("N"&amp;E9))</f>
         <v>378</v>
       </c>
-      <c r="X38" s="8"/>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="R38" s="3"/>
+      <c r="Y38" s="8"/>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>31</v>
       </c>
@@ -7252,9 +7394,9 @@
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
       <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="S39" s="3"/>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>32</v>
       </c>
@@ -7263,7 +7405,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>33</v>
       </c>
@@ -7272,7 +7414,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>34</v>
       </c>
@@ -7281,7 +7423,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>35</v>
       </c>
@@ -7290,7 +7432,7 @@
         <v>31.746031746031747</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>36</v>
       </c>
@@ -7299,7 +7441,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>37</v>
       </c>
@@ -7308,7 +7450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>38</v>
       </c>
@@ -7317,7 +7459,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>39</v>
       </c>
@@ -7326,7 +7468,7 @@
         <v>38.095238095238095</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>40</v>
       </c>
@@ -7335,7 +7477,7 @@
         <v>1.2499999999999997E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>41</v>
       </c>
@@ -7344,17 +7486,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="29"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="57" t="s">
         <v>78</v>
       </c>
       <c r="B51" s="58"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>42</v>
       </c>
@@ -7362,7 +7504,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>43</v>
       </c>
@@ -7370,7 +7512,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>44</v>
       </c>
@@ -7378,7 +7520,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>45</v>
       </c>
@@ -7386,7 +7528,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>46</v>
       </c>
@@ -7394,8 +7536,12 @@
         <f>SUM(B52:B55)</f>
         <v>4000</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D56" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" s="26"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>47</v>
       </c>
@@ -7404,7 +7550,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>48</v>
       </c>
@@ -7413,17 +7559,17 @@
         <v>1260000</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
       <c r="B59" s="36"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="59" t="s">
         <v>79</v>
       </c>
       <c r="B60" s="60"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>49</v>
       </c>
@@ -7431,7 +7577,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>50</v>
       </c>
@@ -7439,7 +7585,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>51</v>
       </c>
@@ -7447,7 +7593,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>52</v>
       </c>
@@ -7455,7 +7601,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>53</v>
       </c>
@@ -7463,36 +7609,40 @@
         <f>SUM(B61:B64)</f>
         <v>4000</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D65" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" s="26"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B66" s="29">
         <f ca="1">ROUND(B67/B65,0)</f>
-        <v>273</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B67" s="36">
         <f ca="1">B15*(B8*12)</f>
-        <v>1092000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1536000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
       <c r="B68" s="36"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="43" t="s">
         <v>80</v>
       </c>
       <c r="B69" s="44"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>56</v>
       </c>
@@ -7501,22 +7651,22 @@
         <v>8000</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B71" s="29">
         <f ca="1">ROUND(B72/B70,0)</f>
-        <v>294</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B72" s="38">
         <f ca="1">B67+B58</f>
-        <v>2352000</v>
+        <v>2796000</v>
       </c>
     </row>
   </sheetData>
@@ -7524,7 +7674,7 @@
     <mergeCell ref="A69:B69"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="K1:Z1"/>
+    <mergeCell ref="K1:AA1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A22:B22"/>

</xml_diff>